<commit_message>
finish setting up effective tax rates
</commit_message>
<xml_diff>
--- a/input_data/admin_data/CHL/gpinter_CHL_2005.xlsx
+++ b/input_data/admin_data/CHL/gpinter_CHL_2005.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
   <si>
     <t>year</t>
   </si>
@@ -195,6 +195,39 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>country</t>
   </si>
   <si>
@@ -375,10 +408,76 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>component</t>
   </si>
   <si>
     <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t/>
@@ -617,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J71"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -625,31 +724,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="E1" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="G1" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="H1" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="I1" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="J1" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
@@ -657,31 +756,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D2">
-        <v>773954.53197344695</v>
+        <v>1471467.0078183601</v>
       </c>
       <c r="E2">
-        <v>0.68000000000000005</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F2">
-        <v>15698.1076740882</v>
+        <v>18581.970827478799</v>
       </c>
       <c r="G2">
-        <v>0.99996184192743298</v>
+        <v>0.99996789090799698</v>
       </c>
       <c r="H2">
-        <v>2418515.6230007899</v>
+        <v>3421906.41941588</v>
       </c>
       <c r="I2">
-        <v>37463.525736000098</v>
+        <v>37493.695954114701</v>
       </c>
       <c r="J2">
-        <v>154.06415048311001</v>
+        <v>184.151963814065</v>
       </c>
     </row>
     <row r="3">
@@ -689,29 +788,29 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D3"/>
       <c r="E3">
-        <v>0.68999999999999995</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F3">
-        <v>59903.802481853803</v>
+        <v>56839.141407220697</v>
       </c>
       <c r="G3">
-        <v>0.99947778861178804</v>
+        <v>0.99971308603806197</v>
       </c>
       <c r="H3">
-        <v>2495323.75517062</v>
+        <v>3502487.6747364001</v>
       </c>
       <c r="I3">
-        <v>83748.377369443697</v>
+        <v>77076.241007109202</v>
       </c>
       <c r="J3">
-        <v>41.6555152058421</v>
+        <v>61.6210517615499</v>
       </c>
     </row>
     <row r="4">
@@ -719,29 +818,29 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="D4"/>
       <c r="E4">
-        <v>0.69999999999999996</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="F4">
-        <v>108323.207947061</v>
+        <v>97771.507598947501</v>
       </c>
       <c r="G4">
-        <v>0.99839570466616001</v>
+        <v>0.99918928060717205</v>
       </c>
       <c r="H4">
-        <v>2575709.60109733</v>
+        <v>3586034.2950712601</v>
       </c>
       <c r="I4">
-        <v>134417.279365311</v>
+        <v>119408.495963077</v>
       </c>
       <c r="J4">
-        <v>23.778003346763001</v>
+        <v>36.677702769818602</v>
       </c>
     </row>
     <row r="5">
@@ -749,29 +848,29 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D5"/>
       <c r="E5">
-        <v>0.70999999999999996</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="F5">
-        <v>161301.196662089</v>
+        <v>141529.27769687699</v>
       </c>
       <c r="G5">
-        <v>0.99665894528544396</v>
+        <v>0.99837778775460595</v>
       </c>
       <c r="H5">
-        <v>2659892.0949501502</v>
+        <v>3672699.94004896</v>
       </c>
       <c r="I5">
-        <v>189827.901896064</v>
+        <v>164644.233817712</v>
       </c>
       <c r="J5">
-        <v>16.490219229571998</v>
+        <v>25.950107283914999</v>
       </c>
     </row>
     <row r="6">
@@ -779,29 +878,29 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D6"/>
       <c r="E6">
-        <v>0.71999999999999997</v>
+        <v>0.60999999999999999</v>
       </c>
       <c r="F6">
-        <v>219208.451023045</v>
+        <v>188269.81389446999</v>
       </c>
       <c r="G6">
-        <v>0.99420624433139604</v>
+        <v>0.99725887558774895</v>
       </c>
       <c r="H6">
-        <v>2748108.6732735098</v>
+        <v>3762650.0863625901</v>
       </c>
       <c r="I6">
-        <v>250364.34868022799</v>
+        <v>212944.449206155</v>
       </c>
       <c r="J6">
-        <v>12.5365087908249</v>
+        <v>19.9854135324723</v>
       </c>
     </row>
     <row r="7">
@@ -809,29 +908,29 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="D7"/>
       <c r="E7">
-        <v>0.72999999999999998</v>
+        <v>0.62</v>
       </c>
       <c r="F7">
-        <v>282442.68822268001</v>
+        <v>238157.761736699</v>
       </c>
       <c r="G7">
-        <v>0.99097137279389302</v>
+        <v>0.99581171810426705</v>
       </c>
       <c r="H7">
-        <v>2840617.7223325199</v>
+        <v>3856063.3926035399</v>
       </c>
       <c r="I7">
-        <v>316438.30190640298</v>
+        <v>264477.46831300302</v>
       </c>
       <c r="J7">
-        <v>10.0573243379307</v>
+        <v>16.191214447449799</v>
       </c>
     </row>
     <row r="8">
@@ -839,29 +938,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="D8"/>
       <c r="E8">
-        <v>0.73999999999999999</v>
+        <v>0.63</v>
       </c>
       <c r="F8">
-        <v>351429.71175540902</v>
+        <v>291365.13898913201</v>
       </c>
       <c r="G8">
-        <v>0.98688278245901195</v>
+        <v>0.99401434536734701</v>
       </c>
       <c r="H8">
-        <v>2937701.5461950698</v>
+        <v>3953133.2824492301</v>
       </c>
       <c r="I8">
-        <v>388489.94954762002</v>
+        <v>319419.013497921</v>
       </c>
       <c r="J8">
-        <v>8.3592862183481795</v>
+        <v>13.5676261620189</v>
       </c>
     </row>
     <row r="9">
@@ -869,29 +968,29 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="D9"/>
       <c r="E9">
-        <v>0.75</v>
+        <v>0.64000000000000001</v>
       </c>
       <c r="F9">
-        <v>426624.19690919801</v>
+        <v>348071.37431248202</v>
       </c>
       <c r="G9">
-        <v>0.98186323759560701</v>
+        <v>0.99184359324174198</v>
       </c>
       <c r="H9">
-        <v>3039670.0100609702</v>
+        <v>4054069.7899201</v>
       </c>
       <c r="I9">
-        <v>466988.58852592303</v>
+        <v>377952.21237061202</v>
       </c>
       <c r="J9">
-        <v>7.1249357914593903</v>
+        <v>11.6472370011116</v>
       </c>
     </row>
     <row r="10">
@@ -899,29 +998,29 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D10"/>
       <c r="E10">
-        <v>0.76000000000000001</v>
+        <v>0.65000000000000002</v>
       </c>
       <c r="F10">
-        <v>508510.08845667198</v>
+        <v>408463.28479576699</v>
       </c>
       <c r="G10">
-        <v>0.97582943884860396</v>
+        <v>0.98927505306814301</v>
       </c>
       <c r="H10">
-        <v>3146865.0692915898</v>
+        <v>4159101.7207072298</v>
       </c>
       <c r="I10">
-        <v>552432.76397891098</v>
+        <v>440267.53968708601</v>
       </c>
       <c r="J10">
-        <v>6.1884024343397597</v>
+        <v>10.1823147282057</v>
       </c>
     </row>
     <row r="11">
@@ -929,29 +1028,29 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="D11"/>
       <c r="E11">
-        <v>0.77000000000000002</v>
+        <v>0.66000000000000003</v>
       </c>
       <c r="F11">
-        <v>597600.45135596802</v>
+        <v>472734.980069254</v>
       </c>
       <c r="G11">
-        <v>0.968691645332875</v>
+        <v>0.98628302173242299</v>
       </c>
       <c r="H11">
-        <v>3259666.4738703999</v>
+        <v>4268479.1966195898</v>
       </c>
       <c r="I11">
-        <v>645349.762642883</v>
+        <v>506562.679179264</v>
       </c>
       <c r="J11">
-        <v>5.4545917200600398</v>
+        <v>9.0293280095208406</v>
       </c>
     </row>
     <row r="12">
@@ -959,29 +1058,29 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="D12"/>
       <c r="E12">
-        <v>0.78000000000000003</v>
+        <v>0.67000000000000004</v>
       </c>
       <c r="F12">
-        <v>694436.56780530198</v>
+        <v>541087.679507719</v>
       </c>
       <c r="G12">
-        <v>0.96035330327294299</v>
+        <v>0.98284045267387299</v>
       </c>
       <c r="H12">
-        <v>3378499.0516534699</v>
+        <v>4382476.66684506</v>
       </c>
       <c r="I12">
-        <v>746294.22498156899</v>
+        <v>577042.29133377201</v>
       </c>
       <c r="J12">
-        <v>4.8650938160282804</v>
+        <v>8.0993835801846803</v>
       </c>
     </row>
     <row r="13">
@@ -989,29 +1088,29 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D13"/>
       <c r="E13">
-        <v>0.79000000000000004</v>
+        <v>0.68000000000000005</v>
       </c>
       <c r="F13">
-        <v>799586.01438745297</v>
+        <v>613729.42814354599</v>
       </c>
       <c r="G13">
-        <v>0.95071069257488805</v>
+        <v>0.97891890847160601</v>
       </c>
       <c r="H13">
-        <v>3503842.1386378501</v>
+        <v>4501396.4910797803</v>
       </c>
       <c r="I13">
-        <v>855845.574220184</v>
+        <v>651917.67254938197</v>
       </c>
       <c r="J13">
-        <v>4.3820703158772396</v>
+        <v>7.33449674182308</v>
       </c>
     </row>
     <row r="14">
@@ -1019,29 +1118,29 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="D14"/>
       <c r="E14">
-        <v>0.80000000000000004</v>
+        <v>0.68999999999999995</v>
       </c>
       <c r="F14">
-        <v>913639.37941217795</v>
+        <v>690874.69666205102</v>
       </c>
       <c r="G14">
-        <v>0.93965260661681604</v>
+        <v>0.9744885157473</v>
       </c>
       <c r="H14">
-        <v>3636241.9668587302</v>
+        <v>4625573.2271614103</v>
       </c>
       <c r="I14">
-        <v>974603.87935196201</v>
+        <v>731406.29137838003</v>
       </c>
       <c r="J14">
-        <v>3.9799531946600601</v>
+        <v>6.6952419150821196</v>
       </c>
     </row>
     <row r="15">
@@ -1049,29 +1148,29 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="D15"/>
       <c r="E15">
-        <v>0.81000000000000005</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="F15">
-        <v>1037205.19208127</v>
+        <v>772743.851772486</v>
       </c>
       <c r="G15">
-        <v>0.92706008549200403</v>
+        <v>0.96951792321962404</v>
       </c>
       <c r="H15">
-        <v>3776328.18199067</v>
+        <v>4755378.79168751</v>
       </c>
       <c r="I15">
-        <v>1103183.6739883199</v>
+        <v>815731.189399831</v>
       </c>
       <c r="J15">
-        <v>3.64086895324257</v>
+        <v>6.1538875796679902</v>
       </c>
     </row>
     <row r="16">
@@ -1079,29 +1178,29 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D16"/>
       <c r="E16">
-        <v>0.81999999999999995</v>
+        <v>0.70999999999999996</v>
       </c>
       <c r="F16">
-        <v>1170902.5338850699</v>
+        <v>859562.48617680406</v>
       </c>
       <c r="G16">
-        <v>0.91280622911654696</v>
+        <v>0.96397426383028295</v>
       </c>
       <c r="H16">
-        <v>3924836.21021302</v>
+        <v>4891228.7090077698</v>
       </c>
       <c r="I16">
-        <v>1242205.14868565</v>
+        <v>905120.23872550495</v>
       </c>
       <c r="J16">
-        <v>3.3519751615793099</v>
+        <v>5.6903701448898403</v>
       </c>
     </row>
     <row r="17">
@@ -1109,29 +1208,29 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D17"/>
       <c r="E17">
-        <v>0.82999999999999996</v>
+        <v>0.71999999999999997</v>
       </c>
       <c r="F17">
-        <v>1315350.6979823599</v>
+        <v>951560.60363636003</v>
       </c>
       <c r="G17">
-        <v>0.89675612413792205</v>
+        <v>0.95782312191601404</v>
       </c>
       <c r="H17">
-        <v>4082638.0373616898</v>
+        <v>5033589.7258035699</v>
       </c>
       <c r="I17">
-        <v>1392282.03764063</v>
+        <v>999805.25695326098</v>
       </c>
       <c r="J17">
-        <v>3.1038399444529299</v>
+        <v>5.2898256890500299</v>
       </c>
     </row>
     <row r="18">
@@ -1139,29 +1238,29 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D18"/>
       <c r="E18">
-        <v>0.83999999999999997</v>
+        <v>0.72999999999999998</v>
       </c>
       <c r="F18">
-        <v>1471155.17988002</v>
+        <v>1048971.66640938</v>
       </c>
       <c r="G18">
-        <v>0.87876692735538597</v>
+        <v>0.95102850639530601</v>
       </c>
       <c r="H18">
-        <v>4250785.2873442601</v>
+        <v>5182989.1505757999</v>
       </c>
       <c r="I18">
-        <v>1554005.47285156</v>
+        <v>1100020.9962595501</v>
       </c>
       <c r="J18">
-        <v>2.8894200594738999</v>
+        <v>4.94101920628336</v>
       </c>
     </row>
     <row r="19">
@@ -1169,29 +1268,29 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D19"/>
       <c r="E19">
-        <v>0.84999999999999998</v>
+        <v>0.73999999999999999</v>
       </c>
       <c r="F19">
-        <v>1638889.28487984</v>
+        <v>1152031.5330423701</v>
       </c>
       <c r="G19">
-        <v>0.85868815775519802</v>
+        <v>0.94355283082517905</v>
       </c>
       <c r="H19">
-        <v>4430570.6083104396</v>
+        <v>5340026.3872802705</v>
       </c>
       <c r="I19">
-        <v>1727923.1781230499</v>
+        <v>1206004.05070096</v>
       </c>
       <c r="J19">
-        <v>2.7033983620408302</v>
+        <v>4.6353126925075703</v>
       </c>
     </row>
     <row r="20">
@@ -1199,29 +1298,29 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="D20"/>
       <c r="E20">
-        <v>0.85999999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="F20">
-        <v>1819070.8693039999</v>
+        <v>1260977.34970881</v>
       </c>
       <c r="G20">
-        <v>0.836362257372948</v>
+        <v>0.93535690088388201</v>
       </c>
       <c r="H20">
-        <v>4623616.85332382</v>
+        <v>5505387.2807434499</v>
       </c>
       <c r="I20">
-        <v>1914513.84760437</v>
+        <v>1317991.7718283001</v>
       </c>
       <c r="J20">
-        <v>2.54174641095367</v>
+        <v>4.3659684149082896</v>
       </c>
     </row>
     <row r="21">
@@ -1229,29 +1328,29 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D21"/>
       <c r="E21">
-        <v>0.87</v>
+        <v>0.76000000000000001</v>
       </c>
       <c r="F21">
-        <v>2012134.5266278</v>
+        <v>1376046.5170553301</v>
       </c>
       <c r="G21">
-        <v>0.81162548320195504</v>
+        <v>0.92639990922300597</v>
       </c>
       <c r="H21">
-        <v>4832009.3922253205</v>
+        <v>5679862.0936149098</v>
       </c>
       <c r="I21">
-        <v>2114157.92175237</v>
+        <v>1436221.35914753</v>
       </c>
       <c r="J21">
-        <v>2.4014345603042</v>
+        <v>4.1276672141647603</v>
       </c>
     </row>
     <row r="22">
@@ -1259,29 +1358,29 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="D22"/>
       <c r="E22">
-        <v>0.88</v>
+        <v>0.77000000000000002</v>
       </c>
       <c r="F22">
-        <v>2218401.6622704398</v>
+        <v>1497475.9517498801</v>
       </c>
       <c r="G22">
-        <v>0.78430917669540001</v>
+        <v>0.91663943650077395</v>
       </c>
       <c r="H22">
-        <v>5058497.0147647299</v>
+        <v>5864368.2125048004</v>
       </c>
       <c r="I22">
-        <v>2327109.4732288602</v>
+        <v>1560929.41820223</v>
       </c>
       <c r="J22">
-        <v>2.2802439706016</v>
+        <v>3.9161685405712099</v>
       </c>
     </row>
     <row r="23">
@@ -1289,29 +1388,29 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="D23"/>
       <c r="E23">
-        <v>0.89000000000000001</v>
+        <v>0.78000000000000003</v>
       </c>
       <c r="F23">
-        <v>2438056.2294777702</v>
+        <v>1625502.0224675899</v>
       </c>
       <c r="G23">
-        <v>0.75424139652109001</v>
+        <v>0.906031455418572</v>
       </c>
       <c r="H23">
-        <v>5306804.9730861699</v>
+        <v>6059979.0667912802</v>
       </c>
       <c r="I23">
-        <v>2553482.5708957901</v>
+        <v>1692352.48774992</v>
       </c>
       <c r="J23">
-        <v>2.17665405289807</v>
+        <v>3.7280661500450898</v>
       </c>
     </row>
     <row r="24">
@@ -1319,29 +1418,29 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="D24"/>
       <c r="E24">
-        <v>0.90000000000000002</v>
+        <v>0.79000000000000004</v>
       </c>
       <c r="F24">
-        <v>2671147.0555913202</v>
+        <v>1760361.8058899699</v>
       </c>
       <c r="G24">
-        <v>0.72124872750234503</v>
+        <v>0.89453033117482095</v>
       </c>
       <c r="H24">
-        <v>5582137.2133052098</v>
+        <v>6267961.2848408697</v>
       </c>
       <c r="I24">
-        <v>2793287.0732533401</v>
+        <v>1830729.3842799801</v>
       </c>
       <c r="J24">
-        <v>2.0897903024921498</v>
+        <v>3.5606096791403798</v>
       </c>
     </row>
     <row r="25">
@@ -1349,29 +1448,29 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="D25"/>
       <c r="E25">
-        <v>0.91000000000000003</v>
+        <v>0.80000000000000004</v>
       </c>
       <c r="F25">
-        <v>2917670.8607359398</v>
+        <v>1902296.7515535399</v>
       </c>
       <c r="G25">
-        <v>0.68515762708419803</v>
+        <v>0.88208880598565398</v>
       </c>
       <c r="H25">
-        <v>5892009.4510887498</v>
+        <v>6489822.8798689097</v>
       </c>
       <c r="I25">
-        <v>3046604.5544779701</v>
+        <v>1976306.7934396099</v>
       </c>
       <c r="J25">
-        <v>2.01942224888333</v>
+        <v>3.4115722873252499</v>
       </c>
     </row>
     <row r="26">
@@ -1379,29 +1478,29 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="D26"/>
       <c r="E26">
-        <v>0.92000000000000004</v>
+        <v>0.81000000000000005</v>
       </c>
       <c r="F26">
-        <v>3177877.5648119398</v>
+        <v>2051560.5912170799</v>
       </c>
       <c r="G26">
-        <v>0.64579349871983904</v>
+        <v>0.86865794560659804</v>
       </c>
       <c r="H26">
-        <v>6247685.0631651003</v>
+        <v>6727376.3581020301</v>
       </c>
       <c r="I26">
-        <v>3314147.6919913902</v>
+        <v>2129350.5244094902</v>
       </c>
       <c r="J26">
-        <v>1.96599300499949</v>
+        <v>3.2791507045429502</v>
       </c>
     </row>
     <row r="27">
@@ -1409,29 +1508,29 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="D27"/>
       <c r="E27">
-        <v>0.93000000000000005</v>
+        <v>0.81999999999999995</v>
       </c>
       <c r="F27">
-        <v>3453186.2533687698</v>
+        <v>2208434.6039559999</v>
       </c>
       <c r="G27">
-        <v>0.60297253760290004</v>
+        <v>0.85418700937020497</v>
       </c>
       <c r="H27">
-        <v>6666761.8304756302</v>
+        <v>6982822.2377516199</v>
       </c>
       <c r="I27">
-        <v>3598899.5703449501</v>
+        <v>2290166.54305099</v>
       </c>
       <c r="J27">
-        <v>1.9306117137388199</v>
+        <v>3.1618877123384999</v>
       </c>
     </row>
     <row r="28">
@@ -1439,29 +1538,29 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D28"/>
       <c r="E28">
-        <v>0.93999999999999995</v>
+        <v>0.82999999999999996</v>
       </c>
       <c r="F28">
-        <v>3748862.2115953499</v>
+        <v>2373255.5633160402</v>
       </c>
       <c r="G28">
-        <v>0.55647239551873395</v>
+        <v>0.83862317728370495</v>
       </c>
       <c r="H28">
-        <v>7178072.2071640799</v>
+        <v>7258860.8080281299</v>
       </c>
       <c r="I28">
-        <v>3911027.6102592298</v>
+        <v>2459138.8826474301</v>
       </c>
       <c r="J28">
-        <v>1.91473353834187</v>
+        <v>3.0586089927397699</v>
       </c>
     </row>
     <row r="29">
@@ -1469,29 +1568,29 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="D29"/>
       <c r="E29">
-        <v>0.94999999999999996</v>
+        <v>0.83999999999999997</v>
       </c>
       <c r="F29">
-        <v>4082255.58630013</v>
+        <v>2546465.6161835399</v>
       </c>
       <c r="G29">
-        <v>0.50593935451066796</v>
+        <v>0.82191101948756495</v>
       </c>
       <c r="H29">
-        <v>7831481.1265450502</v>
+        <v>7558843.4283644203</v>
       </c>
       <c r="I29">
-        <v>4283974.4717862001</v>
+        <v>2636796.8796267798</v>
       </c>
       <c r="J29">
-        <v>1.91842008933178</v>
+        <v>2.9683665784944102</v>
       </c>
     </row>
     <row r="30">
@@ -1499,29 +1598,29 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="D30"/>
       <c r="E30">
-        <v>0.95999999999999996</v>
+        <v>0.84999999999999998</v>
       </c>
       <c r="F30">
-        <v>4511170.9484050302</v>
+        <v>2728700.4522690298</v>
       </c>
       <c r="G30">
-        <v>0.45058759552732403</v>
+        <v>0.80399150878418801</v>
       </c>
       <c r="H30">
-        <v>8718357.7902347501</v>
+        <v>7886979.8649469297</v>
       </c>
       <c r="I30">
-        <v>4835848.5955232903</v>
+        <v>2823934.0110037299</v>
       </c>
       <c r="J30">
-        <v>1.93261525443127</v>
+        <v>2.8903795058884398</v>
       </c>
     </row>
     <row r="31">
@@ -1529,29 +1628,29 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="D31"/>
       <c r="E31">
-        <v>0.96999999999999997</v>
+        <v>0.85999999999999999</v>
       </c>
       <c r="F31">
-        <v>5250263.7179223802</v>
+        <v>2920945.34639929</v>
       </c>
       <c r="G31">
-        <v>0.38810526102644899</v>
+        <v>0.78480022555459905</v>
       </c>
       <c r="H31">
-        <v>10012527.521805201</v>
+        <v>8248625.9973714398</v>
       </c>
       <c r="I31">
-        <v>5943734.1405539</v>
+        <v>3021819.18983133</v>
       </c>
       <c r="J31">
-        <v>1.9070523043683201</v>
+        <v>2.82395766409656</v>
       </c>
     </row>
     <row r="32">
@@ -1559,29 +1658,29 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="D32"/>
       <c r="E32">
-        <v>0.97999999999999998</v>
+        <v>0.87</v>
       </c>
       <c r="F32">
-        <v>6798763.3603604399</v>
+        <v>3124813.99275439</v>
       </c>
       <c r="G32">
-        <v>0.31130831889344701</v>
+        <v>0.76426412672414301</v>
       </c>
       <c r="H32">
-        <v>12046924.2124309</v>
+        <v>8650688.0594899096</v>
       </c>
       <c r="I32">
-        <v>7936203.5883056</v>
+        <v>3232577.6333156601</v>
       </c>
       <c r="J32">
-        <v>1.77192874261066</v>
+        <v>2.7683849597283401</v>
       </c>
     </row>
     <row r="33">
@@ -1589,29 +1688,29 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="D33"/>
       <c r="E33">
-        <v>0.98999999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="F33">
-        <v>9178033.5806487799</v>
+        <v>3343055.2573106699</v>
       </c>
       <c r="G33">
-        <v>0.208767365123596</v>
+        <v>0.74229572637170604</v>
       </c>
       <c r="H33">
-        <v>16157644.8365562</v>
+        <v>9102197.2616710998</v>
       </c>
       <c r="I33">
-        <v>9322560.8922744002</v>
+        <v>3459891.7769707702</v>
       </c>
       <c r="J33">
-        <v>1.7604691347636201</v>
+        <v>2.72271816081</v>
       </c>
     </row>
     <row r="34">
@@ -1619,29 +1718,29 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="D34"/>
       <c r="E34">
-        <v>0.99099999999999999</v>
+        <v>0.89000000000000001</v>
       </c>
       <c r="F34">
-        <v>9473288.0172035508</v>
+        <v>3580496.31157606</v>
       </c>
       <c r="G34">
-        <v>0.19672200521271899</v>
+        <v>0.718782512969114</v>
       </c>
       <c r="H34">
-        <v>16917098.608143099</v>
+        <v>9615134.1239165794</v>
       </c>
       <c r="I34">
-        <v>9642763.5843102206</v>
+        <v>3710327.2992964098</v>
       </c>
       <c r="J34">
-        <v>1.78576842353167</v>
+        <v>2.6854193629050802</v>
       </c>
     </row>
     <row r="35">
@@ -1649,29 +1748,29 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="D35"/>
       <c r="E35">
-        <v>0.99199999999999999</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="F35">
-        <v>9825986.5304180309</v>
+        <v>3845852.5884986902</v>
       </c>
       <c r="G35">
-        <v>0.18426292242949299</v>
+        <v>0.69356735503772704</v>
       </c>
       <c r="H35">
-        <v>17826390.486122198</v>
+        <v>10205614.806378599</v>
       </c>
       <c r="I35">
-        <v>10050961.440246699</v>
+        <v>3995930.3759669499</v>
       </c>
       <c r="J35">
-        <v>1.81420872407443</v>
+        <v>2.6536677034630101</v>
       </c>
     </row>
     <row r="36">
@@ -1679,29 +1778,29 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="D36"/>
       <c r="E36">
-        <v>0.99299999999999999</v>
+        <v>0.91000000000000003</v>
       </c>
       <c r="F36">
-        <v>10306718.439738</v>
+        <v>4155335.2746950602</v>
       </c>
       <c r="G36">
-        <v>0.171276421252714</v>
+        <v>0.66641125602405404</v>
       </c>
       <c r="H36">
-        <v>18937166.064104401</v>
+        <v>10895579.743091</v>
       </c>
       <c r="I36">
-        <v>10657033.465629101</v>
+        <v>4339534.3110632198</v>
       </c>
       <c r="J36">
-        <v>1.8373613458859299</v>
+        <v>2.6220699469047299</v>
       </c>
     </row>
     <row r="37">
@@ -1709,29 +1808,29 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="D37"/>
       <c r="E37">
-        <v>0.99399999999999999</v>
+        <v>0.92000000000000004</v>
       </c>
       <c r="F37">
-        <v>11077972.108498501</v>
+        <v>4540176.4101606598</v>
       </c>
       <c r="G37">
-        <v>0.157506835281745</v>
+        <v>0.63692004563329496</v>
       </c>
       <c r="H37">
-        <v>20317188.1638503</v>
+        <v>11715085.4220945</v>
       </c>
       <c r="I37">
-        <v>11708028.370602701</v>
+        <v>4786160.0063528102</v>
       </c>
       <c r="J37">
-        <v>1.83401690894887</v>
+        <v>2.58031502826119</v>
       </c>
     </row>
     <row r="38">
@@ -1739,29 +1838,29 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="D38"/>
       <c r="E38">
-        <v>0.995</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="F38">
-        <v>12461593.7906783</v>
+        <v>5063188.72468735</v>
       </c>
       <c r="G38">
-        <v>0.14237929498457899</v>
+        <v>0.60439359426929895</v>
       </c>
       <c r="H38">
-        <v>22039020.122499801</v>
+        <v>12704931.910057601</v>
       </c>
       <c r="I38">
-        <v>13413079.1742866</v>
+        <v>5422912.4850392304</v>
       </c>
       <c r="J38">
-        <v>1.76855549079009</v>
+        <v>2.5092748070223498</v>
       </c>
     </row>
     <row r="39">
@@ -1769,29 +1868,29 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D39"/>
       <c r="E39">
-        <v>0.996</v>
+        <v>0.93999999999999995</v>
       </c>
       <c r="F39">
-        <v>14423414.302679799</v>
+        <v>5829768.0496569602</v>
       </c>
       <c r="G39">
-        <v>0.12504871725660099</v>
+        <v>0.56753981191314995</v>
       </c>
       <c r="H39">
-        <v>24195505.359553099</v>
+        <v>13918601.8142273</v>
       </c>
       <c r="I39">
-        <v>15428629.6428816</v>
+        <v>6332420.6792810904</v>
       </c>
       <c r="J39">
-        <v>1.67751579839579</v>
+        <v>2.38750524817987</v>
       </c>
     </row>
     <row r="40">
@@ -1799,29 +1898,29 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="D40"/>
       <c r="E40">
-        <v>0.997</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="F40">
-        <v>16364725.5489957</v>
+        <v>6882607.4832576197</v>
       </c>
       <c r="G40">
-        <v>0.105113916172691</v>
+        <v>0.52450506736478397</v>
       </c>
       <c r="H40">
-        <v>27117797.265110299</v>
+        <v>15435838.041216601</v>
       </c>
       <c r="I40">
-        <v>17212826.736446999</v>
+        <v>7523831.6921866396</v>
       </c>
       <c r="J40">
-        <v>1.6570884237514401</v>
+        <v>2.24273112752183</v>
       </c>
     </row>
     <row r="41">
@@ -1829,29 +1928,29 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D41"/>
       <c r="E41">
-        <v>0.998</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="F41">
-        <v>18334774.741053499</v>
+        <v>8208309.7698113704</v>
       </c>
       <c r="G41">
-        <v>0.082873815462178105</v>
+        <v>0.47337356626955002</v>
       </c>
       <c r="H41">
-        <v>32070282.529441901</v>
+        <v>17413839.628474001</v>
       </c>
       <c r="I41">
-        <v>21928415.199845299</v>
+        <v>8988255.6909340806</v>
       </c>
       <c r="J41">
-        <v>1.7491506158312999</v>
+        <v>2.1214890905456398</v>
       </c>
     </row>
     <row r="42">
@@ -1859,29 +1958,29 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="D42"/>
       <c r="E42">
-        <v>0.999</v>
+        <v>0.96999999999999997</v>
       </c>
       <c r="F42">
-        <v>25500323.093456902</v>
+        <v>9838319.3420156408</v>
       </c>
       <c r="G42">
-        <v>0.054540865277195302</v>
+        <v>0.41228992903421502</v>
       </c>
       <c r="H42">
-        <v>42212149.859038398</v>
+        <v>20222367.607654002</v>
       </c>
       <c r="I42">
-        <v>25755044.139459498</v>
+        <v>11089467.4845476</v>
       </c>
       <c r="J42">
-        <v>1.65535745191674</v>
+        <v>2.0554697306167</v>
       </c>
     </row>
     <row r="43">
@@ -1889,29 +1988,29 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D43"/>
       <c r="E43">
-        <v>0.99909999999999999</v>
+        <v>0.97999999999999998</v>
       </c>
       <c r="F43">
-        <v>26061080.926717401</v>
+        <v>12836749.393365201</v>
       </c>
       <c r="G43">
-        <v>0.051213144710227899</v>
+        <v>0.33692658466002301</v>
       </c>
       <c r="H43">
-        <v>44040717.161213703</v>
+        <v>24788817.6692072</v>
       </c>
       <c r="I43">
-        <v>26596148.4970784</v>
+        <v>15956991.821767099</v>
       </c>
       <c r="J43">
-        <v>1.6899037029605199</v>
+        <v>1.9310821540240899</v>
       </c>
     </row>
     <row r="44">
@@ -1919,29 +2018,29 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="D44"/>
       <c r="E44">
-        <v>0.99919999999999998</v>
+        <v>0.98999999999999999</v>
       </c>
       <c r="F44">
-        <v>27312086.1748343</v>
+        <v>19824918.2044468</v>
       </c>
       <c r="G44">
-        <v>0.047776747945516097</v>
+        <v>0.228483841893908</v>
       </c>
       <c r="H44">
-        <v>46221288.244230203</v>
+        <v>33620643.516647197</v>
       </c>
       <c r="I44">
-        <v>28384497.300480399</v>
+        <v>20370384.7181306</v>
       </c>
       <c r="J44">
-        <v>1.6923382545130901</v>
+        <v>1.69587804448575</v>
       </c>
     </row>
     <row r="45">
@@ -1949,29 +2048,29 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D45"/>
       <c r="E45">
-        <v>0.99929999999999997</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="F45">
-        <v>29603864.503079299</v>
+        <v>20960695.434785899</v>
       </c>
       <c r="G45">
-        <v>0.044109284790012401</v>
+        <v>0.214640252734317</v>
       </c>
       <c r="H45">
-        <v>48769401.236194097</v>
+        <v>35092894.494260199</v>
       </c>
       <c r="I45">
-        <v>30992960.5309259</v>
+        <v>21661596.905954</v>
       </c>
       <c r="J45">
-        <v>1.64739982616531</v>
+        <v>1.6742237681685299</v>
       </c>
     </row>
     <row r="46">
@@ -1979,29 +2078,29 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="D46"/>
       <c r="E46">
-        <v>0.99939999999999996</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="F46">
-        <v>32375974.405340701</v>
+        <v>22426098.5958042</v>
       </c>
       <c r="G46">
-        <v>0.040104791082624297</v>
+        <v>0.19991916365052501</v>
       </c>
       <c r="H46">
-        <v>51732141.353738301</v>
+        <v>36771806.692798398</v>
       </c>
       <c r="I46">
-        <v>33432936.412300099</v>
+        <v>23319516.729209799</v>
       </c>
       <c r="J46">
-        <v>1.59785588863094</v>
+        <v>1.6396880864368599</v>
       </c>
     </row>
     <row r="47">
@@ -2009,29 +2108,29 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="D47"/>
       <c r="E47">
-        <v>0.99950000000000006</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="F47">
-        <v>34141574.878729001</v>
+        <v>24268793.9434806</v>
       </c>
       <c r="G47">
-        <v>0.035785036493546703</v>
+        <v>0.18407136237105001</v>
       </c>
       <c r="H47">
-        <v>55391982.342025101</v>
+        <v>38693562.401882499</v>
       </c>
       <c r="I47">
-        <v>35493175.923250198</v>
+        <v>25259061.955356199</v>
       </c>
       <c r="J47">
-        <v>1.6224202468333</v>
+        <v>1.59437516722074</v>
       </c>
     </row>
     <row r="48">
@@ -2039,29 +2138,29 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="D48"/>
       <c r="E48">
-        <v>0.99960000000000004</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="F48">
-        <v>36844776.967773102</v>
+        <v>26203183.730583701</v>
       </c>
       <c r="G48">
-        <v>0.031199085451597799</v>
+        <v>0.166905457990491</v>
       </c>
       <c r="H48">
-        <v>60366683.9467173</v>
+        <v>40932645.809636898</v>
       </c>
       <c r="I48">
-        <v>39846502.390172303</v>
+        <v>26873530.833267499</v>
       </c>
       <c r="J48">
-        <v>1.6384054651631701</v>
+        <v>1.56212490171038</v>
       </c>
     </row>
     <row r="49">
@@ -2069,29 +2168,29 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="D49"/>
       <c r="E49">
-        <v>0.99970000000000003</v>
+        <v>0.995</v>
       </c>
       <c r="F49">
-        <v>44810540.471221402</v>
+        <v>27486690.263868</v>
       </c>
       <c r="G49">
-        <v>0.026050656087328799</v>
+        <v>0.14864237041157899</v>
       </c>
       <c r="H49">
-        <v>67206744.4655734</v>
+        <v>43744468.804910801</v>
       </c>
       <c r="I49">
-        <v>47967018.241224103</v>
+        <v>28650287.9375991</v>
       </c>
       <c r="J49">
-        <v>1.4997976761457601</v>
+        <v>1.5914782167285599</v>
       </c>
     </row>
     <row r="50">
@@ -2099,29 +2198,29 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="D50"/>
       <c r="E50">
-        <v>0.99980000000000002</v>
+        <v>0.996</v>
       </c>
       <c r="F50">
-        <v>58434608.792323403</v>
+        <v>30379828.581682298</v>
       </c>
       <c r="G50">
-        <v>0.019853002832568301</v>
+        <v>0.12917180954587701</v>
       </c>
       <c r="H50">
-        <v>76826607.577748105</v>
+        <v>47518014.021738701</v>
       </c>
       <c r="I50">
-        <v>66621510.014113203</v>
+        <v>32801530.163291398</v>
       </c>
       <c r="J50">
-        <v>1.3147449630541701</v>
+        <v>1.56413041943199</v>
       </c>
     </row>
     <row r="51">
@@ -2129,29 +2228,29 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C51" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="D51"/>
       <c r="E51">
-        <v>0.99990000000000001</v>
+        <v>0.997</v>
       </c>
       <c r="F51">
-        <v>75454200.621165499</v>
+        <v>34503154.548475303</v>
       </c>
       <c r="G51">
-        <v>0.011245066931704399</v>
+        <v>0.106880089793408</v>
       </c>
       <c r="H51">
-        <v>87031705.141383097</v>
+        <v>52423508.641221099</v>
       </c>
       <c r="I51">
-        <v>76430687.685167506</v>
+        <v>35245473.849380299</v>
       </c>
       <c r="J51">
-        <v>1.15343750811628</v>
+        <v>1.5193830630056899</v>
       </c>
     </row>
     <row r="52">
@@ -2159,29 +2258,29 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="D52"/>
       <c r="E52">
-        <v>0.99990999999999997</v>
+        <v>0.998</v>
       </c>
       <c r="F52">
-        <v>77418632.709575295</v>
+        <v>38115521.007440999</v>
       </c>
       <c r="G52">
-        <v>0.0102575323346791</v>
+        <v>0.082927480824188604</v>
       </c>
       <c r="H52">
-        <v>88209595.969844893</v>
+        <v>61012526.037141599</v>
       </c>
       <c r="I52">
-        <v>78431231.397087604</v>
+        <v>44462167.182465702</v>
       </c>
       <c r="J52">
-        <v>1.1393845755549601</v>
+        <v>1.60072653933369</v>
       </c>
     </row>
     <row r="53">
@@ -2189,29 +2288,29 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="D53"/>
       <c r="E53">
-        <v>0.99992000000000003</v>
+        <v>0.999</v>
       </c>
       <c r="F53">
-        <v>79457120.983980805</v>
+        <v>46970186.601332299</v>
       </c>
       <c r="G53">
-        <v>0.0092441494012303095</v>
+        <v>0.052711263303697402</v>
       </c>
       <c r="H53">
-        <v>89431891.541433394</v>
+        <v>77562884.891817406</v>
       </c>
       <c r="I53">
-        <v>80511867.633481607</v>
+        <v>48701489.101467997</v>
       </c>
       <c r="J53">
-        <v>1.1255365212573401</v>
+        <v>1.65132162556955</v>
       </c>
     </row>
     <row r="54">
@@ -2219,29 +2318,29 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D54"/>
       <c r="E54">
-        <v>0.99992999999999999</v>
+        <v>0.99909999999999999</v>
       </c>
       <c r="F54">
-        <v>81582321.720617995</v>
+        <v>52850974.226271801</v>
       </c>
       <c r="G54">
-        <v>0.0082038832834169396</v>
+        <v>0.049401539820758601</v>
       </c>
       <c r="H54">
-        <v>90706180.671149001</v>
+        <v>80769706.646300405</v>
       </c>
       <c r="I54">
-        <v>82687277.271120906</v>
+        <v>56470536.049368203</v>
       </c>
       <c r="J54">
-        <v>1.1118362257668499</v>
+        <v>1.52825388422358</v>
       </c>
     </row>
     <row r="55">
@@ -2249,29 +2348,29 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="D55"/>
       <c r="E55">
-        <v>0.99994000000000005</v>
+        <v>0.99919999999999998</v>
       </c>
       <c r="F55">
-        <v>83811248.031409502</v>
+        <v>58239986.962877698</v>
       </c>
       <c r="G55">
-        <v>0.0071355094467794797</v>
+        <v>0.045563836647713199</v>
       </c>
       <c r="H55">
-        <v>92042664.571146607</v>
+        <v>83807102.970916495</v>
       </c>
       <c r="I55">
-        <v>84977634.900021404</v>
+        <v>59523497.975600801</v>
       </c>
       <c r="J55">
-        <v>1.0982137449695599</v>
+        <v>1.4389959088475599</v>
       </c>
     </row>
     <row r="56">
@@ -2279,29 +2378,29 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D56"/>
       <c r="E56">
-        <v>0.99995000000000001</v>
+        <v>0.99929999999999997</v>
       </c>
       <c r="F56">
-        <v>86167794.267486796</v>
+        <v>60879779.4685155</v>
       </c>
       <c r="G56">
-        <v>0.0060375426878808104</v>
+        <v>0.041518656044999797</v>
       </c>
       <c r="H56">
-        <v>93455670.505380198</v>
+        <v>87276189.398818001</v>
       </c>
       <c r="I56">
-        <v>87412136.201075196</v>
+        <v>62406633.425693102</v>
       </c>
       <c r="J56">
-        <v>1.0845777276748001</v>
+        <v>1.433582548438</v>
       </c>
     </row>
     <row r="57">
@@ -2309,29 +2408,29 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="D57"/>
       <c r="E57">
-        <v>0.99995999999999996</v>
+        <v>0.99939999999999996</v>
       </c>
       <c r="F57">
-        <v>88687576.327895507</v>
+        <v>64033850.376462102</v>
       </c>
       <c r="G57">
-        <v>0.0049081205759927398</v>
+        <v>0.037277539316313398</v>
       </c>
       <c r="H57">
-        <v>94966554.081447601</v>
+        <v>91421115.394338101</v>
       </c>
       <c r="I57">
-        <v>90036219.389917895</v>
+        <v>65902606.021382198</v>
       </c>
       <c r="J57">
-        <v>1.07079884256096</v>
+        <v>1.42769980029099</v>
       </c>
     </row>
     <row r="58">
@@ -2339,29 +2438,29 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="D58"/>
       <c r="E58">
-        <v>0.99997000000000003</v>
+        <v>0.99950000000000006</v>
       </c>
       <c r="F58">
-        <v>91428438.055923507</v>
+        <v>67917499.354242504</v>
       </c>
       <c r="G58">
-        <v>0.0037447935888126598</v>
+        <v>0.032798838423176498</v>
       </c>
       <c r="H58">
-        <v>96609998.9786136</v>
+        <v>96524817.268928096</v>
       </c>
       <c r="I58">
-        <v>92928904.344247907</v>
+        <v>70297355.897675395</v>
       </c>
       <c r="J58">
-        <v>1.05667340526501</v>
+        <v>1.4212068787379299</v>
       </c>
     </row>
     <row r="59">
@@ -2369,29 +2468,29 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="D59"/>
       <c r="E59">
-        <v>0.99997999999999998</v>
+        <v>0.99960000000000004</v>
       </c>
       <c r="F59">
-        <v>94498018.124603495</v>
+        <v>72906929.382049307</v>
       </c>
       <c r="G59">
-        <v>0.0025440912154069801</v>
+        <v>0.028021473010010199</v>
       </c>
       <c r="H59">
-        <v>98450546.295804903</v>
+        <v>103081682.61173899</v>
       </c>
       <c r="I59">
-        <v>96257422.205220804</v>
+        <v>76123114.516810194</v>
       </c>
       <c r="J59">
-        <v>1.04182657212969</v>
+        <v>1.41388045670621</v>
       </c>
     </row>
     <row r="60">
@@ -2399,29 +2498,359 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="D60"/>
       <c r="E60">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="F60">
+        <v>79744947.353910998</v>
+      </c>
+      <c r="G60">
+        <v>0.022848192595809901</v>
+      </c>
+      <c r="H60">
+        <v>112067871.976726</v>
+      </c>
+      <c r="I60">
+        <v>84543865.108467907</v>
+      </c>
+      <c r="J60">
+        <v>1.4053288101046</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61"/>
+      <c r="E61">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="F61">
+        <v>90217108.910851702</v>
+      </c>
+      <c r="G61">
+        <v>0.017102643109531902</v>
+      </c>
+      <c r="H61">
+        <v>125829875.410855</v>
+      </c>
+      <c r="I61">
+        <v>98982064.186519802</v>
+      </c>
+      <c r="J61">
+        <v>1.3947451534408399</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62"/>
+      <c r="E62">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F62">
+        <v>110646882.667064</v>
+      </c>
+      <c r="G62">
+        <v>0.0103758824237275</v>
+      </c>
+      <c r="H62">
+        <v>152677686.63519099</v>
+      </c>
+      <c r="I62">
+        <v>112316047.45364</v>
+      </c>
+      <c r="J62">
+        <v>1.37986433015557</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" t="s">
+        <v>204</v>
+      </c>
+      <c r="D63"/>
+      <c r="E63">
+        <v>0.99990999999999997</v>
+      </c>
+      <c r="F63">
+        <v>114059447.868644</v>
+      </c>
+      <c r="G63">
+        <v>0.0096125894184724107</v>
+      </c>
+      <c r="H63">
+        <v>157162313.21089599</v>
+      </c>
+      <c r="I63">
+        <v>115970843.49591</v>
+      </c>
+      <c r="J63">
+        <v>1.3778982464643399</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64"/>
+      <c r="E64">
+        <v>0.99992000000000003</v>
+      </c>
+      <c r="F64">
+        <v>117977515.899995</v>
+      </c>
+      <c r="G64">
+        <v>0.0088244586423205408</v>
+      </c>
+      <c r="H64">
+        <v>162311246.92524099</v>
+      </c>
+      <c r="I64">
+        <v>120203141.660385</v>
+      </c>
+      <c r="J64">
+        <v>1.37578118751734</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" t="s">
+        <v>206</v>
+      </c>
+      <c r="D65"/>
+      <c r="E65">
+        <v>0.99992999999999999</v>
+      </c>
+      <c r="F65">
+        <v>122554952.43493</v>
+      </c>
+      <c r="G65">
+        <v>0.00800756542607786</v>
+      </c>
+      <c r="H65">
+        <v>168326690.53454399</v>
+      </c>
+      <c r="I65">
+        <v>125202538.20998199</v>
+      </c>
+      <c r="J65">
+        <v>1.3734793020617899</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66"/>
+      <c r="E66">
+        <v>0.99994000000000005</v>
+      </c>
+      <c r="F66">
+        <v>128024154.797169</v>
+      </c>
+      <c r="G66">
+        <v>0.0071566966159436699</v>
+      </c>
+      <c r="H66">
+        <v>175514049.255265</v>
+      </c>
+      <c r="I66">
+        <v>131264602.804216</v>
+      </c>
+      <c r="J66">
+        <v>1.37094479970077</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67"/>
+      <c r="E67">
+        <v>0.99995000000000001</v>
+      </c>
+      <c r="F67">
+        <v>134758455.573383</v>
+      </c>
+      <c r="G67">
+        <v>0.0062646303847089004</v>
+      </c>
+      <c r="H67">
+        <v>184363938.54553199</v>
+      </c>
+      <c r="I67">
+        <v>138885159.57244599</v>
+      </c>
+      <c r="J67">
+        <v>1.3681066450419299</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68"/>
+      <c r="E68">
+        <v>0.99995999999999996</v>
+      </c>
+      <c r="F68">
+        <v>143410195.908566</v>
+      </c>
+      <c r="G68">
+        <v>0.00532077531467425</v>
+      </c>
+      <c r="H68">
+        <v>195733633.28874201</v>
+      </c>
+      <c r="I68">
+        <v>148987105.19492999</v>
+      </c>
+      <c r="J68">
+        <v>1.36485158568179</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" t="s">
+        <v>210</v>
+      </c>
+      <c r="D69"/>
+      <c r="E69">
+        <v>0.99997000000000003</v>
+      </c>
+      <c r="F69">
+        <v>155267413.17987201</v>
+      </c>
+      <c r="G69">
+        <v>0.0043082680385841902</v>
+      </c>
+      <c r="H69">
+        <v>211315809.31989601</v>
+      </c>
+      <c r="I69">
+        <v>163588802.611388</v>
+      </c>
+      <c r="J69">
+        <v>1.36097977671009</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>140</v>
+      </c>
+      <c r="C70" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70"/>
+      <c r="E70">
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="F70">
+        <v>173426285.44275701</v>
+      </c>
+      <c r="G70">
+        <v>0.0031965285177980602</v>
+      </c>
+      <c r="H70">
+        <v>235179312.67428401</v>
+      </c>
+      <c r="I70">
+        <v>188624838.518305</v>
+      </c>
+      <c r="J70">
+        <v>1.35607651443304</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71"/>
+      <c r="E71">
         <v>0.99999000000000005</v>
       </c>
-      <c r="F60">
-        <v>98155609.501715496</v>
-      </c>
-      <c r="G60">
-        <v>0.00130038220889283</v>
-      </c>
-      <c r="H60">
-        <v>100643670.386365</v>
-      </c>
-      <c r="I60">
-        <v>100643670.38636599</v>
-      </c>
-      <c r="J60">
-        <v>1.0253481272978699</v>
+      <c r="F71">
+        <v>208851794.30037999</v>
+      </c>
+      <c r="G71">
+        <v>0.00191464562463616</v>
+      </c>
+      <c r="H71">
+        <v>281733786.82974303</v>
+      </c>
+      <c r="I71">
+        <v>281733786.82974398</v>
+      </c>
+      <c r="J71">
+        <v>1.34896512511902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>